<commit_message>
xlswrite - xls response desde server
</commit_message>
<xml_diff>
--- a/xlswrite/xls/fechas_horas.xlsx
+++ b/xlswrite/xls/fechas_horas.xlsx
@@ -479,7 +479,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2">
-        <v>41297.52089262731</v>
+        <v>43301.52089262731</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -487,7 +487,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="3">
-        <v>41297.52089262731</v>
+        <v>43301.52089262731</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -495,7 +495,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="4">
-        <v>41297.52089262731</v>
+        <v>43301.52089262731</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -503,7 +503,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="5">
-        <v>41297.52089262731</v>
+        <v>43301.52089262731</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -511,7 +511,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="6">
-        <v>41297.52089262731</v>
+        <v>43301.52089262731</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="7">
-        <v>41297.52089262731</v>
+        <v>43301.52089262731</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -527,7 +527,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="8">
-        <v>41297.52089262731</v>
+        <v>43301.52089262731</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -535,7 +535,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="9">
-        <v>41297.52089262731</v>
+        <v>43301.52089262731</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -543,7 +543,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="10">
-        <v>41297.52089262731</v>
+        <v>43301.52089262731</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -551,7 +551,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="11">
-        <v>41297.52089262731</v>
+        <v>43301.52089262731</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -559,7 +559,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="12">
-        <v>41297.52089262731</v>
+        <v>43301.52089262731</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
@@ -567,7 +567,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="13">
-        <v>41297.52089262731</v>
+        <v>43301.52089262731</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
@@ -575,7 +575,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="14">
-        <v>41297.52089262731</v>
+        <v>43301.52089262731</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
@@ -583,7 +583,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="15">
-        <v>41297.52089262731</v>
+        <v>43301.52089262731</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>

</xml_diff>